<commit_message>
Adds proper loging and error reporting for Rawdata and Attachments modules. More testing is needed, but can be a final submission.
</commit_message>
<xml_diff>
--- a/requests/ECHO_HIV_HI_PBMC_cytoff.xlsx
+++ b/requests/ECHO_HIV_HI_PBMC_cytoff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\Darpa\Programming\submission\requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB19A12-2A81-4D21-893E-334123D0E39D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2631EA83-AC12-4327-A825-4226679EDE42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1022EA94-C927-47D4-994A-3445E7764CD5}"/>
   </bookViews>
@@ -222,7 +222,7 @@
     <t>AS09-13278_6</t>
   </si>
   <si>
-    <t>AS14-03700_6</t>
+    <t>AS14-03700_6A</t>
   </si>
 </sst>
 </file>
@@ -595,14 +595,14 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>